<commit_message>
improvement after review #2
</commit_message>
<xml_diff>
--- a/Workbook1.xlsx
+++ b/Workbook1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="0" windowWidth="25760" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="1800" yWindow="0" windowWidth="25760" windowHeight="16580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,8 +89,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,26 +118,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF8DB4E2"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -247,7 +242,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -275,8 +270,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -294,41 +291,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -336,8 +317,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -351,6 +339,7 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -364,6 +353,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -695,13 +685,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AJ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="AG33" sqref="AG33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="13" width="4.33203125" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" customWidth="1"/>
     <col min="15" max="24" width="4.5" customWidth="1"/>
     <col min="26" max="36" width="4" customWidth="1"/>
   </cols>
@@ -1042,8 +1033,8 @@
       <c r="AF19" s="10"/>
       <c r="AG19" s="10"/>
       <c r="AH19" s="10"/>
-      <c r="AI19" s="30"/>
-      <c r="AJ19" s="30"/>
+      <c r="AI19" s="14"/>
+      <c r="AJ19" s="14"/>
     </row>
     <row r="20" spans="2:36" ht="22" customHeight="1" thickBot="1">
       <c r="B20">
@@ -1078,13 +1069,13 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
-      <c r="AD20" s="30"/>
+      <c r="AD20" s="14"/>
       <c r="AE20" s="10"/>
-      <c r="AF20" s="46"/>
+      <c r="AF20" s="30"/>
       <c r="AG20" s="10"/>
       <c r="AH20" s="10"/>
-      <c r="AI20" s="30"/>
-      <c r="AJ20" s="30"/>
+      <c r="AI20" s="14"/>
+      <c r="AJ20" s="14"/>
     </row>
     <row r="21" spans="2:36" ht="22" customHeight="1" thickBot="1">
       <c r="B21">
@@ -1107,8 +1098,8 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="10"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
@@ -1117,14 +1108,14 @@
         <v>2</v>
       </c>
       <c r="AA21" s="5"/>
-      <c r="AB21" s="30"/>
-      <c r="AC21" s="41" t="s">
+      <c r="AB21" s="14"/>
+      <c r="AC21" s="25" t="s">
         <v>1</v>
       </c>
       <c r="AD21" s="10"/>
-      <c r="AE21" s="44"/>
-      <c r="AF21" s="48"/>
-      <c r="AG21" s="45"/>
+      <c r="AE21" s="28"/>
+      <c r="AF21" s="32"/>
+      <c r="AG21" s="29"/>
       <c r="AH21" s="10"/>
       <c r="AI21" s="10"/>
       <c r="AJ21" s="10"/>
@@ -1136,9 +1127,9 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="16"/>
+      <c r="F22" s="30"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="20"/>
+      <c r="H22" s="30"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1149,9 +1140,9 @@
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
-      <c r="R22" s="16"/>
+      <c r="R22" s="33"/>
       <c r="S22" s="10"/>
-      <c r="T22" s="39"/>
+      <c r="T22" s="23"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
@@ -1160,11 +1151,11 @@
         <v>3</v>
       </c>
       <c r="AA22" s="10"/>
-      <c r="AB22" s="30"/>
+      <c r="AB22" s="14"/>
       <c r="AC22" s="10"/>
       <c r="AD22" s="10"/>
       <c r="AE22" s="10"/>
-      <c r="AF22" s="47"/>
+      <c r="AF22" s="31"/>
       <c r="AG22" s="10"/>
       <c r="AH22" s="10"/>
       <c r="AI22" s="10"/>
@@ -1175,28 +1166,28 @@
         <v>4</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="12"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="10"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="N23">
         <v>4</v>
       </c>
       <c r="O23" s="1"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="43" t="s">
+      <c r="P23" s="33"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="S23" s="38"/>
-      <c r="T23" s="32"/>
-      <c r="U23" s="33"/>
-      <c r="V23" s="30"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="14"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Z23">
@@ -1204,13 +1195,13 @@
       </c>
       <c r="AA23" s="10"/>
       <c r="AB23" s="10"/>
-      <c r="AC23" s="46"/>
+      <c r="AC23" s="30"/>
       <c r="AD23" s="10"/>
       <c r="AE23" s="10"/>
-      <c r="AF23" s="46"/>
+      <c r="AF23" s="30"/>
       <c r="AG23" s="10"/>
       <c r="AH23" s="10"/>
-      <c r="AI23" s="46"/>
+      <c r="AI23" s="30"/>
       <c r="AJ23" s="10"/>
     </row>
     <row r="24" spans="2:36" ht="22" customHeight="1" thickBot="1">
@@ -1218,71 +1209,71 @@
         <v>5</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="25"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="37"/>
       <c r="G24" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="N24">
         <v>5</v>
       </c>
       <c r="O24" s="1"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="37"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="21"/>
       <c r="S24" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="T24" s="37"/>
-      <c r="U24" s="12"/>
-      <c r="V24" s="30"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="14"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Z24">
         <v>5</v>
       </c>
       <c r="AA24" s="10"/>
-      <c r="AB24" s="44"/>
-      <c r="AC24" s="48"/>
-      <c r="AD24" s="45"/>
-      <c r="AE24" s="44"/>
-      <c r="AF24" s="48"/>
-      <c r="AG24" s="45"/>
-      <c r="AH24" s="44"/>
-      <c r="AI24" s="48"/>
-      <c r="AJ24" s="45"/>
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="32"/>
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="28"/>
+      <c r="AF24" s="32"/>
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="28"/>
+      <c r="AI24" s="32"/>
+      <c r="AJ24" s="29"/>
     </row>
     <row r="25" spans="2:36" ht="22" customHeight="1" thickBot="1">
       <c r="B25">
         <v>6</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="12"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="10"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="N25">
         <v>6</v>
       </c>
       <c r="O25" s="1"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="27"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="34"/>
-      <c r="V25" s="30"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="33"/>
+      <c r="S25" s="33"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="18"/>
+      <c r="V25" s="14"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Z25">
@@ -1290,13 +1281,13 @@
       </c>
       <c r="AA25" s="10"/>
       <c r="AB25" s="10"/>
-      <c r="AC25" s="47"/>
+      <c r="AC25" s="31"/>
       <c r="AD25" s="10"/>
       <c r="AE25" s="10"/>
-      <c r="AF25" s="47"/>
+      <c r="AF25" s="31"/>
       <c r="AG25" s="10"/>
       <c r="AH25" s="10"/>
-      <c r="AI25" s="47"/>
+      <c r="AI25" s="31"/>
       <c r="AJ25" s="10"/>
     </row>
     <row r="26" spans="2:36" ht="22" customHeight="1" thickBot="1">
@@ -1306,9 +1297,9 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="21"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1319,9 +1310,9 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="35"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="35"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="33"/>
+      <c r="T26" s="19"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
@@ -1334,7 +1325,7 @@
       <c r="AC26" s="10"/>
       <c r="AD26" s="10"/>
       <c r="AE26" s="10"/>
-      <c r="AF26" s="46"/>
+      <c r="AF26" s="30"/>
       <c r="AG26" s="10"/>
       <c r="AH26" s="10"/>
       <c r="AI26" s="10"/>
@@ -1347,9 +1338,9 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1360,9 +1351,9 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
@@ -1370,16 +1361,16 @@
       <c r="Z27">
         <v>8</v>
       </c>
-      <c r="AA27" s="30"/>
-      <c r="AB27" s="30"/>
+      <c r="AA27" s="14"/>
+      <c r="AB27" s="14"/>
       <c r="AC27" s="10"/>
       <c r="AD27" s="10"/>
-      <c r="AE27" s="44"/>
-      <c r="AF27" s="48"/>
-      <c r="AG27" s="45"/>
+      <c r="AE27" s="28"/>
+      <c r="AF27" s="32"/>
+      <c r="AG27" s="29"/>
       <c r="AH27" s="10"/>
-      <c r="AI27" s="30"/>
-      <c r="AJ27" s="30"/>
+      <c r="AI27" s="14"/>
+      <c r="AJ27" s="14"/>
     </row>
     <row r="28" spans="2:36" ht="22" customHeight="1">
       <c r="B28">
@@ -1411,20 +1402,20 @@
       <c r="Z28">
         <v>9</v>
       </c>
-      <c r="AA28" s="30"/>
-      <c r="AB28" s="30"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="14"/>
       <c r="AC28" s="10"/>
       <c r="AD28" s="10"/>
       <c r="AE28" s="10"/>
-      <c r="AF28" s="47"/>
+      <c r="AF28" s="31"/>
       <c r="AG28" s="10"/>
       <c r="AH28" s="10"/>
-      <c r="AI28" s="30"/>
-      <c r="AJ28" s="30"/>
+      <c r="AI28" s="14"/>
+      <c r="AJ28" s="14"/>
     </row>
     <row r="29" spans="2:36" ht="22" customHeight="1"/>
     <row r="30" spans="2:36" ht="22" customHeight="1">
-      <c r="V30" s="31"/>
+      <c r="V30" s="15"/>
     </row>
     <row r="31" spans="2:36" ht="21" customHeight="1">
       <c r="C31">
@@ -1495,7 +1486,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
-      <c r="F34" s="30"/>
+      <c r="F34" s="14"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
       <c r="I34" s="1"/>
@@ -1510,9 +1501,9 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="20"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="33"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -1523,15 +1514,15 @@
         <v>4</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="43" t="s">
+      <c r="D36" s="14"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G36" s="19"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="12"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="33"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
@@ -1540,15 +1531,15 @@
         <v>5</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="25"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H37" s="28"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
@@ -1557,13 +1548,13 @@
         <v>6</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="12"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
@@ -1574,9 +1565,9 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="21"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -1589,9 +1580,9 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -1614,6 +1605,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>